<commit_message>
se crea la seccion para cargar clientes a granel
</commit_message>
<xml_diff>
--- a/src/views/paginas/Finanzas/archivos/NuevoCliente.xlsx
+++ b/src/views/paginas/Finanzas/archivos/NuevoCliente.xlsx
@@ -2,18 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\ServerJoval\src\views\paginas\Finanzas\archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C631E047-6A24-46F8-A0CF-5F8BC3E7A95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACC1AED-171C-439D-B02D-F964EF398AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{112C8200-8E67-43F8-B4BF-AD833F782847}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Clientes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>DNI</t>
   </si>
   <si>
-    <t>Facturar</t>
-  </si>
-  <si>
     <t>Correo</t>
   </si>
   <si>
@@ -42,10 +39,16 @@
     <t>Nombre</t>
   </si>
   <si>
-    <t>Direccion2</t>
-  </si>
-  <si>
-    <t>LocacionObra</t>
+    <t>MznaYLote</t>
+  </si>
+  <si>
+    <t>CuotasXCobrar</t>
+  </si>
+  <si>
+    <t>MontoCuota</t>
+  </si>
+  <si>
+    <t>AnticipoFinanciero</t>
   </si>
 </sst>
 </file>
@@ -101,16 +104,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}" name="Tabla1" displayName="Tabla1" ref="A1:G2" totalsRowShown="0">
-  <autoFilter ref="A1:G2" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}" name="Tabla1" displayName="Tabla1" ref="A1:H2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{8E528A00-2794-476A-936B-E771A6D11F9F}" name="Nombre"/>
-    <tableColumn id="2" xr3:uid="{7B3E47C8-C58B-4594-835A-A9A3A1C72381}" name="DNI"/>
-    <tableColumn id="3" xr3:uid="{0DE29ACD-DE4C-41BD-822D-FB2DE07BF89E}" name="LocacionObra"/>
+    <tableColumn id="3" xr3:uid="{0DE29ACD-DE4C-41BD-822D-FB2DE07BF89E}" name="DNI"/>
     <tableColumn id="4" xr3:uid="{A0E1F818-7EE2-421B-8AC2-193492055A92}" name="Telefono"/>
     <tableColumn id="5" xr3:uid="{9B876E5B-EBB3-4AB1-B206-B748A7AC4118}" name="Correo"/>
-    <tableColumn id="6" xr3:uid="{6A96E5A5-A177-40B4-BFFD-2C896C2F2D8A}" name="Direccion2"/>
-    <tableColumn id="7" xr3:uid="{31203A6C-FA91-451D-A37B-23A01BE1CA27}" name="Facturar"/>
+    <tableColumn id="6" xr3:uid="{6A96E5A5-A177-40B4-BFFD-2C896C2F2D8A}" name="MznaYLote"/>
+    <tableColumn id="8" xr3:uid="{0A49A181-EA67-4FBE-95AD-8BC71FF197E1}" name="CuotasXCobrar"/>
+    <tableColumn id="9" xr3:uid="{611BB5E5-4545-4552-9873-DF465C9A669D}" name="MontoCuota"/>
+    <tableColumn id="10" xr3:uid="{788F0D6E-A424-47BD-8F41-9E8C652FD76D}" name="AnticipoFinanciero"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -413,40 +417,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFAE7C3-B067-4F00-A6C5-90768CB2152A}">
-  <dimension ref="A1:G1"/>
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H3" sqref="A2:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregado servicio domiciliario en ingreso x lote
</commit_message>
<xml_diff>
--- a/src/views/paginas/Finanzas/archivos/NuevoCliente.xlsx
+++ b/src/views/paginas/Finanzas/archivos/NuevoCliente.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\ServerJoval\src\views\paginas\Finanzas\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACC1AED-171C-439D-B02D-F964EF398AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0A0F03-B5ED-4A8F-9D66-E6DCDCC3080E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{112C8200-8E67-43F8-B4BF-AD833F782847}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{112C8200-8E67-43F8-B4BF-AD833F782847}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>DNI</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>AnticipoFinanciero</t>
+  </si>
+  <si>
+    <t>ServicioDomiciliario</t>
   </si>
 </sst>
 </file>
@@ -104,9 +107,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}" name="Tabla1" displayName="Tabla1" ref="A1:H2" insertRow="1" totalsRowShown="0">
-  <autoFilter ref="A1:H2" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}" name="Tabla1" displayName="Tabla1" ref="A1:I2" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A1:I2" xr:uid="{67A9BF03-516A-475C-8883-6179B1CD2774}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{8E528A00-2794-476A-936B-E771A6D11F9F}" name="Nombre"/>
     <tableColumn id="3" xr3:uid="{0DE29ACD-DE4C-41BD-822D-FB2DE07BF89E}" name="DNI"/>
     <tableColumn id="4" xr3:uid="{A0E1F818-7EE2-421B-8AC2-193492055A92}" name="Telefono"/>
@@ -115,6 +118,7 @@
     <tableColumn id="8" xr3:uid="{0A49A181-EA67-4FBE-95AD-8BC71FF197E1}" name="CuotasXCobrar"/>
     <tableColumn id="9" xr3:uid="{611BB5E5-4545-4552-9873-DF465C9A669D}" name="MontoCuota"/>
     <tableColumn id="10" xr3:uid="{788F0D6E-A424-47BD-8F41-9E8C652FD76D}" name="AnticipoFinanciero"/>
+    <tableColumn id="2" xr3:uid="{2CD4C72B-C7B2-4150-9C79-2D427D4C8E2A}" name="ServicioDomiciliario"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -418,10 +422,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BFAE7C3-B067-4F00-A6C5-90768CB2152A}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="A2:H3"/>
+      <selection activeCell="J4" sqref="H1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -434,9 +438,10 @@
     <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -460,6 +465,9 @@
       </c>
       <c r="H1" t="s">
         <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>